<commit_message>
Updated dcp int test example.
</commit_message>
<xml_diff>
--- a/examples/spreadsheets/current/filled/dcp_integration_test_metadata_1_SS2_bundle.xlsx
+++ b/examples/spreadsheets/current/filled/dcp_integration_test_metadata_1_SS2_bundle.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/examples/spreadsheets/current/filled/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4D260279-BD3D-C744-9232-E4B3DC7AF79A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7A6DD067-5C01-7142-8849-B3E05DA6B6A1}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24660" yWindow="460" windowWidth="26540" windowHeight="16580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="860" yWindow="580" windowWidth="26540" windowHeight="16580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -2715,8 +2715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AV6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
-      <selection activeCell="AS6" sqref="AS6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3246,7 +3246,7 @@
   <dimension ref="A1:AI6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3653,8 +3653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AE6"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4020,7 +4020,7 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4211,8 +4211,8 @@
       <c r="A6" s="8" t="s">
         <v>528</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>511</v>
+      <c r="B6" t="s">
+        <v>516</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>530</v>
@@ -4237,8 +4237,8 @@
       <c r="A7" s="8" t="s">
         <v>529</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>511</v>
+      <c r="B7" t="s">
+        <v>516</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>530</v>

</xml_diff>